<commit_message>
Se agrego la columna entorno
</commit_message>
<xml_diff>
--- a/static/data/data_tests.xlsx
+++ b/static/data/data_tests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\tomcat\webapps\sb-admin-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\tomcat\webapps\Salesforce_login\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBD6F34-368B-4671-9C0B-A4026D960CA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A3A001-9444-44A2-B36A-39FB7CA363BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3109759D-9FE3-40E7-9A20-0CE398D0EEE8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>squad</t>
   </si>
@@ -90,18 +90,6 @@
     <t>JDR</t>
   </si>
   <si>
-    <t>alex@bcp.com.pe</t>
-  </si>
-  <si>
-    <t>alex2@bcp.com.pe</t>
-  </si>
-  <si>
-    <t>alex3@bcp.com.pe</t>
-  </si>
-  <si>
-    <t>juan1@bcp.com.pe</t>
-  </si>
-  <si>
     <t>delegado1</t>
   </si>
   <si>
@@ -127,6 +115,21 @@
   </si>
   <si>
     <t>juan2</t>
+  </si>
+  <si>
+    <t>alex@bcp.com.pe.uat</t>
+  </si>
+  <si>
+    <t>alex2@bcp.com.pe.uat</t>
+  </si>
+  <si>
+    <t>alex3@bcp.com.pe.int</t>
+  </si>
+  <si>
+    <t>juan1@bcp.com.pe.uat</t>
+  </si>
+  <si>
+    <t>juan1@bcp.com.pe.int</t>
   </si>
 </sst>
 </file>
@@ -498,7 +501,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,13 +540,13 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -560,13 +563,13 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
@@ -583,13 +586,13 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
         <v>7</v>
@@ -606,13 +609,13 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
@@ -626,16 +629,16 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
         <v>7</v>
@@ -644,11 +647,11 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{A4195118-A6E7-4FBF-8795-1D2416CF80E4}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{EB1A3D45-256D-407E-97F3-509E450ABF09}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{19C8814D-587D-48FA-8D0D-1D8B6E3A7E1C}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{A0B85C40-DC9D-4AA7-8B8D-1D157ADD92BD}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{35C197B5-A087-4FAB-B772-FBAF9D01857A}"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{EB1A3D45-256D-407E-97F3-509E450ABF09}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{19C8814D-587D-48FA-8D0D-1D8B6E3A7E1C}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{A0B85C40-DC9D-4AA7-8B8D-1D157ADD92BD}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{35C197B5-A087-4FAB-B772-FBAF9D01857A}"/>
+    <hyperlink ref="F2" r:id="rId5" xr:uid="{A4195118-A6E7-4FBF-8795-1D2416CF80E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>

</xml_diff>

<commit_message>
Agregamos la condicional ternaria
</commit_message>
<xml_diff>
--- a/static/data/data_tests.xlsx
+++ b/static/data/data_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\tomcat\webapps\Salesforce_login\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A3A001-9444-44A2-B36A-39FB7CA363BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31794C7-85EB-432D-A552-8AE289FA11E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3109759D-9FE3-40E7-9A20-0CE398D0EEE8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>squad</t>
   </si>
@@ -42,12 +42,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>mayorista</t>
-  </si>
-  <si>
-    <t>alex</t>
-  </si>
-  <si>
     <t>pass123</t>
   </si>
   <si>
@@ -57,18 +51,6 @@
     <t>pass345</t>
   </si>
   <si>
-    <t>alex2</t>
-  </si>
-  <si>
-    <t>alex3</t>
-  </si>
-  <si>
-    <t>bdn</t>
-  </si>
-  <si>
-    <t>juan1</t>
-  </si>
-  <si>
     <t>puesto</t>
   </si>
   <si>
@@ -81,42 +63,6 @@
     <t>delegado</t>
   </si>
   <si>
-    <t>EDN</t>
-  </si>
-  <si>
-    <t>ADN</t>
-  </si>
-  <si>
-    <t>JDR</t>
-  </si>
-  <si>
-    <t>delegado1</t>
-  </si>
-  <si>
-    <t>delegado2</t>
-  </si>
-  <si>
-    <t>delegado3</t>
-  </si>
-  <si>
-    <t>delegado4</t>
-  </si>
-  <si>
-    <t>manager1</t>
-  </si>
-  <si>
-    <t>manager2</t>
-  </si>
-  <si>
-    <t>manager3</t>
-  </si>
-  <si>
-    <t>manager4</t>
-  </si>
-  <si>
-    <t>juan2</t>
-  </si>
-  <si>
     <t>alex@bcp.com.pe.uat</t>
   </si>
   <si>
@@ -130,6 +76,48 @@
   </si>
   <si>
     <t>juan1@bcp.com.pe.int</t>
+  </si>
+  <si>
+    <t>Mayorista</t>
+  </si>
+  <si>
+    <t>Negocio</t>
+  </si>
+  <si>
+    <t>Ejecutivo de Negocio</t>
+  </si>
+  <si>
+    <t>Analista de Negocio</t>
+  </si>
+  <si>
+    <t>Jefe de Riesgo</t>
+  </si>
+  <si>
+    <t>Funcionario de Negocio</t>
+  </si>
+  <si>
+    <t>Po - Banca Negocio</t>
+  </si>
+  <si>
+    <t>Alex Mejia</t>
+  </si>
+  <si>
+    <t>Susana Flores</t>
+  </si>
+  <si>
+    <t>Juan Ruiz</t>
+  </si>
+  <si>
+    <t>Pedro Montex</t>
+  </si>
+  <si>
+    <t>Jorge Olivares</t>
+  </si>
+  <si>
+    <t>Manager de prueba</t>
+  </si>
+  <si>
+    <t>Iveth Mattos</t>
   </si>
 </sst>
 </file>
@@ -501,26 +489,29 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -531,117 +522,96 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se modifica data_test password
</commit_message>
<xml_diff>
--- a/static/data/data_tests.xlsx
+++ b/static/data/data_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyecto BCP\SF_Access_Control\Salesforce_Control_Access\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362258D0-2245-4095-884F-22C037EFB05E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E76865-3352-46DA-ACD3-D4A7AE6A9C30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3109759D-9FE3-40E7-9A20-0CE398D0EEE8}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t>spavlich@bcp.com.pe.int</t>
   </si>
   <si>
-    <t>Mayorista2021*.*</t>
-  </si>
-  <si>
     <t>STEPHANY DE JESUS ALFARO</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>Gerencia de División de Riesgos</t>
+  </si>
+  <si>
+    <t>testPassword</t>
   </si>
 </sst>
 </file>
@@ -178,6 +178,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DEBCB23-C631-49EC-9ED4-1C37E35A8998}" name="Tabla1" displayName="Tabla1" ref="A1:G6" totalsRowShown="0">
+  <autoFilter ref="A1:G6" xr:uid="{CA69B20A-7E80-491E-8F25-9C9A41A2A9D1}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{F8C94C36-1158-4DDC-9445-2B947FA5C04F}" name="squad"/>
+    <tableColumn id="2" xr3:uid="{35C827CA-603D-4C59-BDCA-8BC142FCA234}" name="puesto"/>
+    <tableColumn id="3" xr3:uid="{AD218B7A-7DA5-4CF5-A233-3438F8E8B85D}" name="nombreUsuario"/>
+    <tableColumn id="4" xr3:uid="{EF1FC143-09EF-4056-A66A-4CAAFF014015}" name="manager"/>
+    <tableColumn id="5" xr3:uid="{6D6F03DB-294F-4A49-916C-68FA0346DC9B}" name="delegado"/>
+    <tableColumn id="6" xr3:uid="{D69959B1-AC04-4DF3-ADA8-0507EA065587}" name="user" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="7" xr3:uid="{E9470D9E-537C-46F2-AA80-250C5A6B96CD}" name="password"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -480,13 +496,18 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -529,7 +550,7 @@
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -537,19 +558,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -557,19 +578,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -577,16 +598,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -594,16 +615,16 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -617,5 +638,8 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
+  <tableParts count="1">
+    <tablePart r:id="rId7"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>